<commit_message>
Update Placement Information (2022-23) (Responses) (5).xlsx
</commit_message>
<xml_diff>
--- a/2023/Master/Placement Information (2022-23) (Responses) (5).xlsx
+++ b/2023/Master/Placement Information (2022-23) (Responses) (5).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\cv\2023\Master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9932A20B-3BB5-489A-975B-390F11A84747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC09BBF-5E27-4CD3-9D15-44229120D8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,13 +1046,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1289,12 +1292,13 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="18.88671875" customWidth="1"/>
     <col min="10" max="10" width="18.88671875" hidden="1" customWidth="1"/>
@@ -1378,7 +1382,9 @@
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="6">
+        <v>7721839072</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1420,15 +1426,17 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C2,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/chaitaliahirrao07112000@gmail.com.pdf</v>
+        <f t="shared" ref="X2:X42" si="0">HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/Master/",A2,".pdf"))</f>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Ahirrao Chaitali Sanjay.pdf</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="6">
+        <v>8485860669</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
@@ -1442,15 +1450,17 @@
         <v>37</v>
       </c>
       <c r="X3" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C3,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/awareadityaonly1@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Aware Aditya Bapurao.pdf</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="6">
+        <v>9370373159</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1506,15 +1516,17 @@
         <v>0.69159999999999999</v>
       </c>
       <c r="X4" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C4,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/mayuribari0310@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Bari Mayuri Rajesh.pdf</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="6">
+        <v>9370860580</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1552,15 +1564,17 @@
         <v>2</v>
       </c>
       <c r="X5" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C5,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/harshalbhandarkar001@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Bhandarkar Harshal Suresh.pdf</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="6">
+        <v>7498591791</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
@@ -1607,15 +1621,17 @@
         <v>52.33</v>
       </c>
       <c r="X6" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C6,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/jayeshchaudhari7585@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Chaudhari Jayesh Suresh.pdf</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="6">
+        <v>7083344262</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>60</v>
       </c>
@@ -1648,8 +1664,8 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C7,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/kbdesale999@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Desale Kalyani Bhausaheb.pdf</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1718,8 +1734,8 @@
         <v>0.70830000000000004</v>
       </c>
       <c r="X8" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C8,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/fulpagarepradip677@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Fulpagare Pradip Shantaram.pdf</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1768,8 +1784,8 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C9,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/aakashgaikwad0330@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Gaikwad Aakash Pandurang.pdf</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1832,8 +1848,8 @@
         <v>63.16</v>
       </c>
       <c r="X10" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C10,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/sachinghogare1762@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Ghogare Sachin Nanasaheb.pdf</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1890,8 +1906,8 @@
         <v>67.67</v>
       </c>
       <c r="X11" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C11,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/prachigore408@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Gore Prachi Ganpat.pdf</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1943,8 +1959,8 @@
       </c>
       <c r="W12" s="1"/>
       <c r="X12" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C12,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/anjalijadhav4112000@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Jadhav Anjali Sakarchand.pdf</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1974,15 +1990,17 @@
         <v>105</v>
       </c>
       <c r="X13" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C13,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/jamadarchetana264@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Jamadhar Chetana Sunilsing.pdf</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1">
+        <v>8080664723</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>106</v>
       </c>
@@ -2044,15 +2062,17 @@
         <v>56.11</v>
       </c>
       <c r="X14" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C14,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/priyadkhairnar15@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Khairnar Priyanka Devidas.pdf</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1">
+        <v>7057685423</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>116</v>
       </c>
@@ -2099,15 +2119,17 @@
         <v>50.33</v>
       </c>
       <c r="X15" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C15,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/vivekslohar@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Lohar Vivek Sahebrao.pdf</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>7620698045</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>121</v>
       </c>
@@ -2157,15 +2179,17 @@
         <v>6.04</v>
       </c>
       <c r="X16" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C16,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/dhanashrimahajan019@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Mahajan Dhanashri Vikas.pdf</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>9834149987</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>125</v>
       </c>
@@ -2221,15 +2245,17 @@
         <v>73.33</v>
       </c>
       <c r="X17" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C17,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/mahajankanchan558@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Mahajan Kanchan Jayant.pdf</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1">
+        <v>9923296898</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>131</v>
       </c>
@@ -2268,15 +2294,17 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C18,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/lalitmarathe52000@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Marathe Lalit Dattatray.pdf</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1">
+        <v>7046197557</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>139</v>
       </c>
@@ -2293,15 +2321,17 @@
         <v>49</v>
       </c>
       <c r="X19" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C19,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/Vishalmotirale111@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Motirale Vishal Rajendra.pdf</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1">
+        <v>9370679120</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>143</v>
       </c>
@@ -2318,15 +2348,17 @@
         <v>59</v>
       </c>
       <c r="X20" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C20,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/komalnikam0801@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Nikam Komal Dada.pdf</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1">
+        <v>7841048009</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>145</v>
       </c>
@@ -2343,15 +2375,17 @@
         <v>57</v>
       </c>
       <c r="X21" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C21,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/vikrantnikam007@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Nikam Vikrant Dipak.pdf</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>8484886534</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>148</v>
       </c>
@@ -2396,15 +2430,17 @@
         <v>0.56499999999999995</v>
       </c>
       <c r="X22" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C22,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/samiyaa.khanam@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Pathan Samiya Khanam Z..pdf</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1">
+        <v>9146294790</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>151</v>
       </c>
@@ -2460,15 +2496,17 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="X23" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C23,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/patilabhishek151089@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Abhishek Balmukund.pdf</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1">
+        <v>9422387915</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>160</v>
       </c>
@@ -2515,15 +2553,17 @@
         <v>57.66</v>
       </c>
       <c r="X24" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C24,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/patilbhavesh1572000@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Bhavesh Pramod.pdf</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>7218083102</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>166</v>
       </c>
@@ -2585,15 +2625,17 @@
         <v>65.16</v>
       </c>
       <c r="X25" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C25,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/dikshpatil7890@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Diksha Dilip.pdf</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1">
+        <v>7083216462</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>173</v>
       </c>
@@ -2655,15 +2697,17 @@
         <v>60</v>
       </c>
       <c r="X26" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C26,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/dp7083216462@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Divya Dipak.pdf</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1">
+        <v>7057789236</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>182</v>
       </c>
@@ -2693,15 +2737,17 @@
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C27,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/hemangipatil558@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Hemangi Ravindra.pdf</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1">
+        <v>9665783941</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>186</v>
       </c>
@@ -2754,8 +2800,8 @@
         <v>64.5</v>
       </c>
       <c r="X28" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C28,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/hemantppatil2000@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Hemant Prakash.pdf</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -2801,15 +2847,17 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C29,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/nikitapatil7028@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Nikita Sharad.pdf</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1">
+        <v>8999267583</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>197</v>
       </c>
@@ -2862,15 +2910,17 @@
         <v>59.83</v>
       </c>
       <c r="X30" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C30,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/npofficial399398@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Nishant Nana.pdf</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1">
+        <v>9405660772</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>205</v>
       </c>
@@ -2914,15 +2964,17 @@
         <v>57.08</v>
       </c>
       <c r="X31" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C31,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/parudpatil12@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Parag Dilip.pdf</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1">
+        <v>9075347494</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>211</v>
       </c>
@@ -2945,15 +2997,17 @@
         <v>215</v>
       </c>
       <c r="X32" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C32,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/rahuld.patil2401@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Rahul Dineshbhai.pdf</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1">
+        <v>7378672969</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>216</v>
       </c>
@@ -2997,15 +3051,17 @@
         <v>69.16</v>
       </c>
       <c r="X33" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C33,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/104sopanpatil@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Sopan Raman.pdf</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1">
+        <v>9370986862</v>
+      </c>
       <c r="C34" s="1" t="s">
         <v>219</v>
       </c>
@@ -3058,15 +3114,17 @@
         <v>61.35</v>
       </c>
       <c r="X34" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C34,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/vaishnavipatil1143@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Vaishnavi Pradip.pdf</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="1">
+        <v>9518961293</v>
+      </c>
       <c r="C35" s="1" t="s">
         <v>225</v>
       </c>
@@ -3116,15 +3174,17 @@
         <v>78.66</v>
       </c>
       <c r="X35" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C35,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/pvaishnavi808@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Patil Vaishnavi Sharad.pdf</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="1">
+        <v>7038260888</v>
+      </c>
       <c r="C36" s="1" t="s">
         <v>230</v>
       </c>
@@ -3174,15 +3234,17 @@
         <v>63.5</v>
       </c>
       <c r="X36" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C36,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/prasanna291199@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Pawar Prasanna Deepak.pdf</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="1">
+        <v>8668260246</v>
+      </c>
       <c r="C37" s="1" t="s">
         <v>236</v>
       </c>
@@ -3238,15 +3300,17 @@
         <v>0.68330000000000002</v>
       </c>
       <c r="X37" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C37,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/puranikyashashri@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Puranik Yashashri Madhav.pdf</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1">
+        <v>8459370635</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>242</v>
       </c>
@@ -3296,15 +3360,17 @@
         <v>48.835000000000001</v>
       </c>
       <c r="X38" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C38,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/atulsalunke7110@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Salunke Atul Dilip.pdf</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="1">
+        <v>9359004454</v>
+      </c>
       <c r="C39" s="1" t="s">
         <v>248</v>
       </c>
@@ -3357,15 +3423,17 @@
         <v>69.66</v>
       </c>
       <c r="X39" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C39,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/chetansalunke352000@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Salunke Chetan Rajaram.pdf</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="1">
+        <v>9359764318</v>
+      </c>
       <c r="C40" s="1" t="s">
         <v>253</v>
       </c>
@@ -3421,15 +3489,17 @@
         <v>53</v>
       </c>
       <c r="X40" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C40,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/ksapkal2000@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Sapkal Komal Ramesh.pdf</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="1">
+        <v>9370859629</v>
+      </c>
       <c r="C41" s="1" t="s">
         <v>261</v>
       </c>
@@ -3446,15 +3516,17 @@
         <v>27</v>
       </c>
       <c r="X41" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C41,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/pranits1999@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Sonawane Pranit Ramesh.pdf</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="1">
+        <v>7378778184</v>
+      </c>
       <c r="C42" s="1" t="s">
         <v>264</v>
       </c>
@@ -3507,15 +3579,17 @@
         <v>0.60829999999999995</v>
       </c>
       <c r="X42" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C42,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/suryawanshih456@gmail.com.pdf</v>
+        <f t="shared" si="0"/>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Suryawanshi Hitesh Ananda.pdf</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1">
+        <v>8149226221</v>
+      </c>
       <c r="C43" s="1" t="s">
         <v>273</v>
       </c>
@@ -3565,8 +3639,8 @@
         <v>0.62170000000000003</v>
       </c>
       <c r="X43" s="5" t="str">
-        <f>HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/master/",C43,".pdf"))</f>
-        <v>https://kbcnmustats.github.io/cv/2023/master/bhanujayeola10@gmail.com.pdf</v>
+        <f t="shared" ref="X43" si="1">HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/Master/",A43,".pdf"))</f>
+        <v>https://kbcnmustats.github.io/cv/2023/Master/Yeola Bhanuja Bharat.pdf</v>
       </c>
     </row>
   </sheetData>
@@ -3574,7 +3648,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W43">
     <sortCondition ref="A2:A43"/>
   </sortState>
-  <conditionalFormatting sqref="A1:B1048576">
+  <conditionalFormatting sqref="A1:B43 A76:B1048576 A44:A75">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>